<commit_message>
Add notes on high level initial approach and adjust schema designs
</commit_message>
<xml_diff>
--- a/SQL Schema Design.xlsx
+++ b/SQL Schema Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseaschmidt/Documents/Galvanize_Coding_Bootcamp/latitude_SDC_chelsea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474B313C-C93F-FD44-8DF3-571019AC3F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681F5E21-1EB4-1941-A534-954C585B07CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3800" yWindow="-21140" windowWidth="38380" windowHeight="21140" xr2:uid="{3315975D-35F4-C84C-9F96-683F0BF39893}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="57">
   <si>
     <t>SQL Database Schema Design</t>
   </si>
@@ -81,12 +81,6 @@
   </si>
   <si>
     <t>Data Type</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>AUTO INCREMENT</t>
   </si>
   <si>
     <t>guests</t>
@@ -832,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE12132-7C42-A948-8F0A-3C567E761234}">
-  <dimension ref="B2:U37"/>
+  <dimension ref="B2:R37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -846,31 +840,28 @@
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="3.5" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5" customWidth="1"/>
-    <col min="15" max="15" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.5" customWidth="1"/>
-    <col min="26" max="26" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="3.5" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5" customWidth="1"/>
+    <col min="13" max="13" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.5" customWidth="1"/>
+    <col min="23" max="23" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D2" s="25" t="s">
         <v>1</v>
       </c>
@@ -886,11 +877,8 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D3" s="24" t="s">
         <v>0</v>
       </c>
@@ -906,13 +894,10 @@
       <c r="N3" s="24"/>
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-    </row>
-    <row r="5" spans="2:19" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:16" ht="21" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -920,38 +905,29 @@
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>19</v>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>2</v>
@@ -962,38 +938,29 @@
       <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
+      <c r="I6" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="10"/>
       <c r="D7" s="4" t="s">
@@ -1003,29 +970,26 @@
       <c r="F7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="I7" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>23</v>
+      <c r="H7" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="4"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
       <c r="D8" s="4" t="s">
@@ -1035,25 +999,22 @@
       <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4" t="s">
+      <c r="H8" s="12"/>
+      <c r="I8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="M8" s="8"/>
+      <c r="N8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="10"/>
       <c r="D9" s="4" t="s">
@@ -1063,57 +1024,46 @@
       <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="4"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="H9" s="12"/>
+      <c r="I9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" s="4"/>
-      <c r="O10" s="8"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="H10" s="12"/>
+      <c r="I10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="J11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11" s="4"/>
-      <c r="O11" s="8"/>
-    </row>
-    <row r="12" spans="2:19" ht="21" x14ac:dyDescent="0.25">
+      <c r="I11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="2:16" ht="21" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="2" t="s">
@@ -1125,23 +1075,19 @@
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M12" s="4"/>
-      <c r="O12" s="8"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="I12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
       <c r="C13" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>2</v>
@@ -1152,61 +1098,53 @@
       <c r="F13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M13" s="4"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="I13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
       <c r="C14" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="J14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M14" s="4"/>
-      <c r="O14" s="8"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="I14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C15" s="8"/>
       <c r="D15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="J15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M15" s="4"/>
-      <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="I15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C16" s="8"/>
       <c r="D16" s="4" t="s">
         <v>10</v>
@@ -1215,18 +1153,16 @@
       <c r="F16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="J16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M16" s="4"/>
-      <c r="O16" s="8"/>
-    </row>
-    <row r="17" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="I16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C17" s="8"/>
       <c r="D17" s="4" t="s">
         <v>11</v>
@@ -1235,166 +1171,153 @@
       <c r="F17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="J17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M17" s="4"/>
-      <c r="O17" s="8"/>
-    </row>
-    <row r="18" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="I17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="3:18" ht="21" x14ac:dyDescent="0.25">
       <c r="C18" s="8"/>
       <c r="D18" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="J18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M18" s="4"/>
-      <c r="O18" s="8"/>
-    </row>
-    <row r="19" spans="3:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="I18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C19" s="8"/>
       <c r="D19" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="J19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M19" s="4"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="I19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="N19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C20" s="8"/>
       <c r="D20" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="J20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" s="4"/>
-      <c r="O20" s="8"/>
+      <c r="I20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="P20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="3:21" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C21" s="8"/>
       <c r="D21" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="J21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M21" s="4"/>
-      <c r="O21" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q21" s="4" t="s">
+      <c r="I21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S21" s="4"/>
-    </row>
-    <row r="22" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="P21" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C22" s="8"/>
       <c r="D22" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="J22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M22" s="4"/>
-      <c r="O22" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S22" s="4"/>
-    </row>
-    <row r="23" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="I22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C23" s="11"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -1404,124 +1327,121 @@
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="9"/>
-    </row>
-    <row r="24" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="T24" s="3" t="s">
+      <c r="L23" s="15"/>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q24" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R25" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="T25" s="5" t="s">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q26" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="Q28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U25" s="5" t="s">
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R29" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="Q32" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R32" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R33" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="17:18" ht="170" x14ac:dyDescent="0.2">
+      <c r="Q36" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R36" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="T26" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="U26" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="T27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="U27" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="3:21" ht="85" x14ac:dyDescent="0.2">
-      <c r="T28" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="U28" s="7" t="s">
+    <row r="37" spans="17:18" ht="136" x14ac:dyDescent="0.2">
+      <c r="Q37" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R37" s="7" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="T29" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="U29" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="T30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="U30" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="T31" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U31" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="T32" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U32" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="20:21" x14ac:dyDescent="0.2">
-      <c r="T33" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="U33" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="20:21" x14ac:dyDescent="0.2">
-      <c r="T34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="U34" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="20:21" x14ac:dyDescent="0.2">
-      <c r="T35" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="U35" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="20:21" ht="170" x14ac:dyDescent="0.2">
-      <c r="T36" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="U36" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="20:21" ht="136" x14ac:dyDescent="0.2">
-      <c r="T37" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="U37" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D3:S3"/>
-    <mergeCell ref="D2:S2"/>
+    <mergeCell ref="D3:P3"/>
+    <mergeCell ref="D2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pseudocode data generation script for SQL CSV files
</commit_message>
<xml_diff>
--- a/SQL Schema Design.xlsx
+++ b/SQL Schema Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseaschmidt/Documents/Galvanize_Coding_Bootcamp/latitude_SDC_chelsea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681F5E21-1EB4-1941-A534-954C585B07CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86B0E0B-FA25-5B45-BDFC-C9D0152D4D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3800" yWindow="-21140" windowWidth="38380" windowHeight="21140" xr2:uid="{3315975D-35F4-C84C-9F96-683F0BF39893}"/>
   </bookViews>
@@ -829,7 +829,7 @@
   <dimension ref="B2:R37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="D2" sqref="D2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Convert users CSV generation pseudocode to code
</commit_message>
<xml_diff>
--- a/SQL Schema Design.xlsx
+++ b/SQL Schema Design.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseaschmidt/Documents/Galvanize_Coding_Bootcamp/latitude_SDC_chelsea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86B0E0B-FA25-5B45-BDFC-C9D0152D4D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4789E132-262F-2A45-B7D5-D144C53A876B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3800" yWindow="-21140" windowWidth="38380" windowHeight="21140" xr2:uid="{3315975D-35F4-C84C-9F96-683F0BF39893}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="58">
   <si>
     <t>SQL Database Schema Design</t>
   </si>
@@ -225,12 +225,20 @@
   <si>
     <t>&lt;--</t>
   </si>
+  <si>
+    <t>VARCHAR(8)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,6 +272,13 @@
     <font>
       <b/>
       <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -466,10 +481,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -512,8 +528,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -826,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE12132-7C42-A948-8F0A-3C567E761234}">
-  <dimension ref="B2:R37"/>
+  <dimension ref="B2:V37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:P2"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,7 +859,7 @@
     <col min="3" max="3" width="3.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="3.5" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
@@ -861,7 +881,7 @@
     <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D2" s="25" t="s">
         <v>1</v>
       </c>
@@ -878,7 +898,7 @@
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D3" s="24" t="s">
         <v>0</v>
       </c>
@@ -895,7 +915,7 @@
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
     </row>
-    <row r="5" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="21" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>53</v>
       </c>
@@ -924,19 +944,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="22" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>2</v>
@@ -945,7 +965,7 @@
         <v>13</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M6" s="23" t="s">
         <v>55</v>
@@ -957,18 +977,18 @@
         <v>13</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="10"/>
       <c r="D7" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>56</v>
@@ -980,20 +1000,22 @@
         <v>12</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M7" s="8"/>
       <c r="N7" s="4" t="s">
         <v>39</v>
       </c>
       <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
       <c r="D8" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
@@ -1012,18 +1034,13 @@
         <v>40</v>
       </c>
       <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="H9" s="12"/>
       <c r="I9" s="4" t="s">
         <v>22</v>
@@ -1034,7 +1051,7 @@
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
       <c r="H10" s="12"/>
@@ -1047,7 +1064,7 @@
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="13"/>
@@ -1063,18 +1080,9 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="I12" s="4" t="s">
         <v>27</v>
       </c>
@@ -1084,19 +1092,17 @@
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:21" ht="21" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>7</v>
+      <c r="C13" s="8"/>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>25</v>
@@ -1107,18 +1113,20 @@
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
-      <c r="C14" s="20" t="s">
-        <v>56</v>
+      <c r="C14" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="I14" s="4" t="s">
         <v>28</v>
       </c>
@@ -1127,14 +1135,21 @@
         <v>7</v>
       </c>
       <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C15" s="8"/>
-      <c r="D15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="U14" s="26"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C15" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="I15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1143,8 +1158,9 @@
         <v>7</v>
       </c>
       <c r="M15" s="8"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="U15" s="26"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C16" s="8"/>
       <c r="D16" s="4" t="s">
         <v>10</v>
@@ -1161,8 +1177,9 @@
         <v>7</v>
       </c>
       <c r="M16" s="8"/>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U16" s="26"/>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C17" s="8"/>
       <c r="D17" s="4" t="s">
         <v>11</v>
@@ -1179,8 +1196,14 @@
         <v>7</v>
       </c>
       <c r="M17" s="8"/>
-    </row>
-    <row r="18" spans="3:18" ht="21" x14ac:dyDescent="0.25">
+      <c r="U17" s="26">
+        <v>10000000</v>
+      </c>
+      <c r="V17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" ht="21" x14ac:dyDescent="0.25">
       <c r="C18" s="8"/>
       <c r="D18" s="4" t="s">
         <v>16</v>
@@ -1206,8 +1229,15 @@
       <c r="P18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U18" s="27">
+        <f>U17*0.5</f>
+        <v>5000000</v>
+      </c>
+      <c r="V18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C19" s="8"/>
       <c r="D19" s="4" t="s">
         <v>17</v>
@@ -1231,10 +1261,17 @@
         <v>13</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="U19" s="28">
+        <f>3*U17</f>
+        <v>30000000</v>
+      </c>
+      <c r="V19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C20" s="8"/>
       <c r="D20" s="4" t="s">
         <v>18</v>
@@ -1260,10 +1297,16 @@
         <v>12</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="U20" s="26">
+        <v>27</v>
+      </c>
+      <c r="V20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C21" s="8"/>
       <c r="D21" s="4" t="s">
         <v>19</v>
@@ -1289,10 +1332,17 @@
         <v>12</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="U21" s="28">
+        <f>7*U17</f>
+        <v>70000000</v>
+      </c>
+      <c r="V21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="8"/>
       <c r="D22" s="4" t="s">
         <v>20</v>
@@ -1316,8 +1366,12 @@
       <c r="P22" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="U22" s="28">
+        <f>SUM(U17:U21)</f>
+        <v>115000027</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="11"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -1329,12 +1383,12 @@
       <c r="K23" s="14"/>
       <c r="L23" s="15"/>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q24" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q25" s="5" t="s">
         <v>48</v>
       </c>
@@ -1342,7 +1396,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q26" s="6" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1404,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q27" s="6" t="s">
         <v>9</v>
       </c>
@@ -1358,7 +1412,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="3:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:22" ht="85" x14ac:dyDescent="0.2">
       <c r="Q28" s="6" t="s">
         <v>44</v>
       </c>
@@ -1366,7 +1420,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q29" s="6" t="s">
         <v>10</v>
       </c>
@@ -1374,7 +1428,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q30" s="6" t="s">
         <v>11</v>
       </c>
@@ -1382,7 +1436,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q31" s="6" t="s">
         <v>16</v>
       </c>
@@ -1390,7 +1444,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q32" s="6" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Reorganize and add files for seed2.0 script
</commit_message>
<xml_diff>
--- a/SQL Schema Design.xlsx
+++ b/SQL Schema Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseaschmidt/Documents/Galvanize_Coding_Bootcamp/latitude_SDC_chelsea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4789E132-262F-2A45-B7D5-D144C53A876B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE84604-0A90-BE42-86F2-65D9876890D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3800" yWindow="-21140" windowWidth="38380" windowHeight="21140" xr2:uid="{3315975D-35F4-C84C-9F96-683F0BF39893}"/>
   </bookViews>
@@ -235,8 +235,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -522,15 +522,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -882,38 +882,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
     </row>
     <row r="5" spans="2:21" ht="21" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
@@ -1135,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="M14" s="8"/>
-      <c r="U14" s="26"/>
+      <c r="U14" s="24"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C15" s="20" t="s">
@@ -1158,7 +1158,7 @@
         <v>7</v>
       </c>
       <c r="M15" s="8"/>
-      <c r="U15" s="26"/>
+      <c r="U15" s="24"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C16" s="8"/>
@@ -1177,7 +1177,7 @@
         <v>7</v>
       </c>
       <c r="M16" s="8"/>
-      <c r="U16" s="26"/>
+      <c r="U16" s="24"/>
     </row>
     <row r="17" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C17" s="8"/>
@@ -1196,7 +1196,7 @@
         <v>7</v>
       </c>
       <c r="M17" s="8"/>
-      <c r="U17" s="26">
+      <c r="U17" s="24">
         <v>10000000</v>
       </c>
       <c r="V17" t="s">
@@ -1229,7 +1229,7 @@
       <c r="P18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U18" s="27">
+      <c r="U18" s="25">
         <f>U17*0.5</f>
         <v>5000000</v>
       </c>
@@ -1263,7 +1263,7 @@
       <c r="P19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U19" s="28">
+      <c r="U19" s="26">
         <f>3*U17</f>
         <v>30000000</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="P20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U20" s="26">
+      <c r="U20" s="24">
         <v>27</v>
       </c>
       <c r="V20" t="s">
@@ -1334,7 +1334,7 @@
       <c r="P21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U21" s="28">
+      <c r="U21" s="26">
         <f>7*U17</f>
         <v>70000000</v>
       </c>
@@ -1366,7 +1366,7 @@
       <c r="P22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U22" s="28">
+      <c r="U22" s="26">
         <f>SUM(U17:U21)</f>
         <v>115000027</v>
       </c>

</xml_diff>

<commit_message>
Update 0-padding from 3 to 8 and save work before large data generation
</commit_message>
<xml_diff>
--- a/SQL Schema Design.xlsx
+++ b/SQL Schema Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseaschmidt/Documents/Galvanize_Coding_Bootcamp/latitude_SDC_chelsea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE84604-0A90-BE42-86F2-65D9876890D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACF4B1A-DDE5-C246-859B-83958EBFAB7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3800" yWindow="-21140" windowWidth="38380" windowHeight="21140" xr2:uid="{3315975D-35F4-C84C-9F96-683F0BF39893}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>image</t>
   </si>
   <si>
-    <t>VARCHAR</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
@@ -226,7 +223,10 @@
     <t>&lt;--</t>
   </si>
   <si>
-    <t>VARCHAR(8)</t>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>CHAR(8)</t>
   </si>
 </sst>
 </file>
@@ -849,7 +849,7 @@
   <dimension ref="B2:V37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -917,67 +917,67 @@
     </row>
     <row r="5" spans="2:21" ht="21" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="N5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="M6" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
@@ -988,27 +988,27 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="M7" s="8"/>
       <c r="N7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
@@ -1019,23 +1019,23 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
@@ -1043,11 +1043,11 @@
       <c r="C9" s="10"/>
       <c r="H9" s="12"/>
       <c r="I9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M9" s="8"/>
     </row>
@@ -1056,11 +1056,11 @@
       <c r="C10" s="10"/>
       <c r="H10" s="12"/>
       <c r="I10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M10" s="8"/>
     </row>
@@ -1072,11 +1072,11 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="I11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M11" s="8"/>
     </row>
@@ -1084,11 +1084,11 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="I12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M12" s="8"/>
     </row>
@@ -1096,66 +1096,66 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="I13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M13" s="8"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
       <c r="C14" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M14" s="8"/>
       <c r="U14" s="24"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C15" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="I15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M15" s="8"/>
       <c r="U15" s="24"/>
@@ -1163,18 +1163,18 @@
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C16" s="8"/>
       <c r="D16" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M16" s="8"/>
       <c r="U16" s="24"/>
@@ -1182,189 +1182,189 @@
     <row r="17" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C17" s="8"/>
       <c r="D17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M17" s="8"/>
       <c r="U17" s="24">
         <v>10000000</v>
       </c>
       <c r="V17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="3:22" ht="21" x14ac:dyDescent="0.25">
       <c r="C18" s="8"/>
       <c r="D18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M18" s="8"/>
       <c r="N18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="U18" s="25">
         <f>U17*0.5</f>
         <v>5000000</v>
       </c>
       <c r="V18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C19" s="8"/>
       <c r="D19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M19" s="8"/>
       <c r="N19" s="4" t="s">
         <v>2</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="U19" s="26">
         <f>3*U17</f>
         <v>30000000</v>
       </c>
       <c r="V19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C20" s="8"/>
       <c r="D20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M20" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P20" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="U20" s="24">
         <v>27</v>
       </c>
       <c r="V20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C21" s="8"/>
       <c r="D21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M21" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N21" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="U21" s="26">
         <f>7*U17</f>
         <v>70000000</v>
       </c>
       <c r="V21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="8"/>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="U22" s="26">
         <f>SUM(U17:U21)</f>
@@ -1385,15 +1385,15 @@
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="R25" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="R25" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="3:22" x14ac:dyDescent="0.2">
@@ -1401,95 +1401,95 @@
         <v>2</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q27" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="3:22" ht="85" x14ac:dyDescent="0.2">
       <c r="Q28" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R28" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q29" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R29" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q30" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q31" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R31" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="3:22" x14ac:dyDescent="0.2">
       <c r="Q32" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R32" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="17:18" x14ac:dyDescent="0.2">
       <c r="Q33" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R33" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="17:18" x14ac:dyDescent="0.2">
       <c r="Q34" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R34" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="17:18" x14ac:dyDescent="0.2">
       <c r="Q35" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R35" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="17:18" ht="170" x14ac:dyDescent="0.2">
       <c r="Q36" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R36" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="17:18" ht="136" x14ac:dyDescent="0.2">
       <c r="Q37" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R37" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Decouple room data seeding from listing data seeding to save memory
</commit_message>
<xml_diff>
--- a/SQL Schema Design.xlsx
+++ b/SQL Schema Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseaschmidt/Documents/Galvanize_Coding_Bootcamp/latitude_SDC_chelsea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACF4B1A-DDE5-C246-859B-83958EBFAB7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0119B6-1AB2-9F4D-926E-60FF972E5961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3800" yWindow="-21140" windowWidth="38380" windowHeight="21140" xr2:uid="{3315975D-35F4-C84C-9F96-683F0BF39893}"/>
+    <workbookView xWindow="-4520" yWindow="-21140" windowWidth="38380" windowHeight="21140" xr2:uid="{3315975D-35F4-C84C-9F96-683F0BF39893}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,8 +285,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -525,6 +539,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -849,7 +864,7 @@
   <dimension ref="B2:V37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -882,38 +897,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="5" spans="2:21" ht="21" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
@@ -1239,11 +1254,11 @@
     </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C19" s="8"/>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
+      <c r="E19" s="27"/>
+      <c r="F19" s="27" t="s">
         <v>6</v>
       </c>
       <c r="I19" s="4" t="s">
@@ -1273,11 +1288,11 @@
     </row>
     <row r="20" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C20" s="8"/>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="E20" s="27"/>
+      <c r="F20" s="27" t="s">
         <v>6</v>
       </c>
       <c r="I20" s="4" t="s">

</xml_diff>